<commit_message>
Skip columns whose names don't exist
Actually there are sundry changes that were not accurately tracked. See diff.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/Taraba/test_services_excel.xlsx
+++ b/tests/testthat/testdata/Taraba/test_services_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admn\Documents\2-Biz\DevSolutions\clientele\JHPIEGO\jGBV\tests\testthat\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admn\Documents\2-Biz\DevSolutions\clientele\JHPIEGO\jGBV\tests\testthat\testdata\Taraba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2BAEFB3-0D12-48FD-8164-404844809633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22A73FC-C31B-4826-BABA-22EFCC872F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_excel" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="22">
   <si>
     <t>agegp</t>
   </si>
@@ -78,11 +78,20 @@
   <si>
     <t>s/n</t>
   </si>
+  <si>
+    <t>rem1</t>
+  </si>
+  <si>
+    <t>rem2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -917,14 +926,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -932,19 +943,25 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -952,19 +969,25 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
       <c r="F2">
+        <v>99</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -972,19 +995,25 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>43739</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
+        <v>99</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -992,19 +1021,25 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
+        <v>99</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1012,239 +1047,300 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
+        <v>99</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
       <c r="F6">
+        <v>7979</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>43739</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7979</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
+        <v>7979</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7979</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="E10" t="s">
+        <v>7</v>
       </c>
       <c r="F10">
+        <v>119119</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>43739</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119119</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
+        <v>119119</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>43739</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>8</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1252,19 +1348,25 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
+      <c r="E17" t="s">
+        <v>7</v>
       </c>
       <c r="F17">
+        <v>99</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1272,19 +1374,25 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>43739</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
       <c r="F18">
+        <v>99</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1292,19 +1400,25 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
       <c r="F19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1312,239 +1426,303 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
       <c r="F20">
+        <v>99</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+      <c r="E21" t="s">
+        <v>7</v>
       </c>
       <c r="F21">
+        <v>7979</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>43739</v>
       </c>
-      <c r="E22">
+      <c r="F22">
+        <v>7979</v>
+      </c>
+      <c r="G22">
         <v>3</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
       <c r="F23">
+        <v>7979</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
       <c r="F24">
+        <v>7979</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
         <v>11</v>
       </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
+      <c r="E25" t="s">
+        <v>7</v>
       </c>
       <c r="F25">
+        <v>119119</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>43739</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
       <c r="F26">
+        <v>119119</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
       <c r="F27">
+        <v>119119</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
         <v>11</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>9</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
       <c r="F28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119119</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>43739</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
+      <c r="F30" s="1"/>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
         <v>12</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>8</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>2</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1552,19 +1730,25 @@
         <v>14</v>
       </c>
       <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
+      <c r="E32" t="s">
+        <v>7</v>
       </c>
       <c r="F32">
+        <v>99</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1572,19 +1756,25 @@
         <v>14</v>
       </c>
       <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>43739</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
       <c r="F33">
+        <v>99</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1592,19 +1782,25 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>8</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
       <c r="F34">
+        <v>99</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1612,259 +1808,326 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>9</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
       <c r="F35">
+        <v>99</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>14</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
         <v>10</v>
       </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36">
+        <v>7979</v>
+      </c>
+      <c r="G36">
         <v>6</v>
       </c>
-      <c r="F36">
+      <c r="H36">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>14</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>43739</v>
       </c>
-      <c r="E37">
+      <c r="F37">
+        <v>7979</v>
+      </c>
+      <c r="G37">
         <v>4</v>
       </c>
-      <c r="F37">
+      <c r="H37">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
         <v>10</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>8</v>
       </c>
-      <c r="E38">
+      <c r="F38">
+        <v>7979</v>
+      </c>
+      <c r="G38">
         <v>5</v>
       </c>
-      <c r="F38">
+      <c r="H38">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
         <v>10</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>9</v>
       </c>
-      <c r="E39">
+      <c r="F39">
+        <v>7979</v>
+      </c>
+      <c r="G39">
         <v>5</v>
       </c>
-      <c r="F39">
+      <c r="H39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
         <v>11</v>
       </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40">
+        <v>119119</v>
+      </c>
+      <c r="G40">
         <v>3</v>
       </c>
-      <c r="F40">
+      <c r="H40">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>43739</v>
       </c>
-      <c r="E41">
+      <c r="F41">
+        <v>119119</v>
+      </c>
+      <c r="G41">
         <v>6</v>
       </c>
-      <c r="F41">
+      <c r="H41">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>14</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
         <v>11</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>8</v>
       </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
       <c r="F42">
+        <v>119119</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>14</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
         <v>11</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>9</v>
       </c>
-      <c r="E43">
+      <c r="F43">
+        <v>119119</v>
+      </c>
+      <c r="G43">
         <v>2</v>
       </c>
-      <c r="F43">
+      <c r="H43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>14</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
         <v>12</v>
       </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44">
         <v>4</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>43739</v>
       </c>
-      <c r="E45">
+      <c r="F45" s="1"/>
+      <c r="G45">
         <v>3</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
         <v>12</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>8</v>
       </c>
-      <c r="E46">
+      <c r="G46">
         <v>2</v>
       </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>14</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>9</v>
       </c>
-      <c r="E47">
+      <c r="G47">
         <v>4</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1872,19 +2135,25 @@
         <v>15</v>
       </c>
       <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48">
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>99</v>
+      </c>
+      <c r="G48">
         <v>2</v>
       </c>
-      <c r="F48">
+      <c r="H48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1892,19 +2161,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>43739</v>
       </c>
-      <c r="E49">
+      <c r="F49">
+        <v>99</v>
+      </c>
+      <c r="G49">
         <v>3</v>
       </c>
-      <c r="F49">
+      <c r="H49">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1912,19 +2187,25 @@
         <v>15</v>
       </c>
       <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
         <v>6</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>8</v>
       </c>
-      <c r="E50">
+      <c r="F50">
+        <v>99</v>
+      </c>
+      <c r="G50">
         <v>3</v>
       </c>
-      <c r="F50">
+      <c r="H50">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1932,259 +2213,326 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>9</v>
       </c>
-      <c r="E51">
+      <c r="F51">
+        <v>99</v>
+      </c>
+      <c r="G51">
         <v>4</v>
       </c>
-      <c r="F51">
+      <c r="H51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
         <v>10</v>
       </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52">
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52">
+        <v>7979</v>
+      </c>
+      <c r="G52">
         <v>9</v>
       </c>
-      <c r="F52">
+      <c r="H52">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>43739</v>
       </c>
-      <c r="E53">
+      <c r="F53">
+        <v>7979</v>
+      </c>
+      <c r="G53">
         <v>6</v>
       </c>
-      <c r="F53">
+      <c r="H53">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>15</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
         <v>10</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>8</v>
       </c>
-      <c r="E54">
+      <c r="F54">
+        <v>7979</v>
+      </c>
+      <c r="G54">
         <v>4</v>
       </c>
-      <c r="F54">
+      <c r="H54">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>15</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
         <v>10</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>9</v>
       </c>
-      <c r="E55">
+      <c r="F55">
+        <v>7979</v>
+      </c>
+      <c r="G55">
         <v>3</v>
       </c>
-      <c r="F55">
+      <c r="H55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>15</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56">
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56">
+        <v>119119</v>
+      </c>
+      <c r="G56">
         <v>9</v>
       </c>
-      <c r="F56">
+      <c r="H56">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>43739</v>
       </c>
-      <c r="E57">
+      <c r="F57">
+        <v>119119</v>
+      </c>
+      <c r="G57">
         <v>8</v>
       </c>
-      <c r="F57">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
         <v>11</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>8</v>
       </c>
-      <c r="E58">
+      <c r="F58">
+        <v>119119</v>
+      </c>
+      <c r="G58">
         <v>3</v>
       </c>
-      <c r="F58">
+      <c r="H58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
         <v>11</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>9</v>
       </c>
-      <c r="E59">
+      <c r="F59">
+        <v>119119</v>
+      </c>
+      <c r="G59">
         <v>4</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
         <v>12</v>
       </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60">
+      <c r="E60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60">
         <v>5</v>
       </c>
-      <c r="F60">
+      <c r="H60">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>15</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>43739</v>
       </c>
-      <c r="E61">
+      <c r="F61" s="1"/>
+      <c r="G61">
         <v>6</v>
       </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>15</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
         <v>12</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>8</v>
       </c>
-      <c r="E62">
+      <c r="G62">
         <v>2</v>
       </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>15</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63" t="s">
         <v>12</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>9</v>
       </c>
-      <c r="E63">
+      <c r="G63">
         <v>5</v>
       </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2192,19 +2540,25 @@
         <v>16</v>
       </c>
       <c r="C64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" t="s">
         <v>6</v>
       </c>
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64">
+      <c r="E64" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64">
+        <v>99</v>
+      </c>
+      <c r="G64">
         <v>5</v>
       </c>
-      <c r="F64">
+      <c r="H64">
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2212,19 +2566,25 @@
         <v>16</v>
       </c>
       <c r="C65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>43739</v>
       </c>
-      <c r="E65">
+      <c r="F65">
+        <v>99</v>
+      </c>
+      <c r="G65">
         <v>4</v>
       </c>
-      <c r="F65">
+      <c r="H65">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2232,19 +2592,25 @@
         <v>16</v>
       </c>
       <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
         <v>6</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>8</v>
       </c>
-      <c r="E66">
+      <c r="F66">
+        <v>99</v>
+      </c>
+      <c r="G66">
         <v>2</v>
       </c>
-      <c r="F66">
+      <c r="H66">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2252,239 +2618,300 @@
         <v>16</v>
       </c>
       <c r="C67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D67" t="s">
         <v>6</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>9</v>
       </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
       <c r="F67">
+        <v>99</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>16</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
         <v>10</v>
       </c>
-      <c r="D68" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68">
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68">
+        <v>7979</v>
+      </c>
+      <c r="G68">
         <v>17</v>
       </c>
-      <c r="F68">
+      <c r="H68">
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>43739</v>
       </c>
-      <c r="E69">
+      <c r="F69">
+        <v>7979</v>
+      </c>
+      <c r="G69">
         <v>3</v>
       </c>
-      <c r="F69">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>16</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
         <v>10</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>8</v>
       </c>
-      <c r="E70">
+      <c r="F70">
+        <v>7979</v>
+      </c>
+      <c r="G70">
         <v>5</v>
       </c>
-      <c r="F70">
+      <c r="H70">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>16</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
         <v>11</v>
       </c>
-      <c r="D71" t="s">
-        <v>7</v>
-      </c>
-      <c r="E71">
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71">
+        <v>119119</v>
+      </c>
+      <c r="G71">
         <v>6</v>
       </c>
-      <c r="F71">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>16</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>43739</v>
       </c>
-      <c r="E72">
+      <c r="F72">
+        <v>119119</v>
+      </c>
+      <c r="G72">
         <v>4</v>
       </c>
-      <c r="F72">
+      <c r="H72">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>16</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
         <v>11</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>8</v>
       </c>
-      <c r="E73">
+      <c r="F73">
+        <v>119119</v>
+      </c>
+      <c r="G73">
         <v>2</v>
       </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
         <v>11</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E74" t="s">
         <v>9</v>
       </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
       <c r="F74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119119</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>16</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
         <v>12</v>
       </c>
-      <c r="D75" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75">
+      <c r="E75" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75">
         <v>3</v>
       </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>16</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="s">
         <v>12</v>
       </c>
-      <c r="D76" s="1">
+      <c r="E76" s="1">
         <v>43739</v>
       </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="1"/>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>16</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="s">
         <v>12</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>8</v>
       </c>
-      <c r="E77">
-        <v>1</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
         <v>12</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>9</v>
       </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2492,19 +2919,25 @@
         <v>17</v>
       </c>
       <c r="C79" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" t="s">
         <v>6</v>
       </c>
-      <c r="D79" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
+      <c r="E79" t="s">
+        <v>7</v>
       </c>
       <c r="F79">
+        <v>99</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2512,19 +2945,25 @@
         <v>17</v>
       </c>
       <c r="C80" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" t="s">
         <v>6</v>
       </c>
-      <c r="D80" s="1">
+      <c r="E80" s="1">
         <v>43739</v>
       </c>
-      <c r="E80">
+      <c r="F80">
+        <v>99</v>
+      </c>
+      <c r="G80">
         <v>2</v>
       </c>
-      <c r="F80">
+      <c r="H80">
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2532,175 +2971,224 @@
         <v>17</v>
       </c>
       <c r="C81" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" t="s">
         <v>6</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>9</v>
       </c>
-      <c r="E81">
-        <v>1</v>
-      </c>
       <c r="F81">
+        <v>99</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>17</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
         <v>10</v>
       </c>
-      <c r="D82" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82">
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82">
+        <v>7979</v>
+      </c>
+      <c r="G82">
         <v>2</v>
       </c>
-      <c r="F82">
+      <c r="H82">
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>17</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
         <v>10</v>
       </c>
-      <c r="D83" s="1">
+      <c r="E83" s="1">
         <v>43739</v>
       </c>
-      <c r="E83">
-        <v>1</v>
-      </c>
       <c r="F83">
+        <v>7979</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>17</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
         <v>10</v>
       </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>8</v>
       </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
       <c r="F84">
+        <v>7979</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>17</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
         <v>10</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>9</v>
       </c>
-      <c r="E85">
-        <v>1</v>
-      </c>
       <c r="F85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7979</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>17</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
         <v>11</v>
       </c>
-      <c r="D86" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86">
-        <v>1</v>
+      <c r="E86" t="s">
+        <v>7</v>
       </c>
       <c r="F86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119119</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>17</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="1">
+      <c r="E87" s="1">
         <v>43739</v>
       </c>
-      <c r="E87">
-        <v>1</v>
-      </c>
       <c r="F87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119119</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>17</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
         <v>12</v>
       </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88">
+      <c r="E88" t="s">
+        <v>7</v>
+      </c>
+      <c r="G88">
         <v>2</v>
       </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>17</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" t="s">
         <v>12</v>
       </c>
-      <c r="D89" s="1">
+      <c r="E89" s="1">
         <v>43739</v>
       </c>
-      <c r="E89">
-        <v>1</v>
-      </c>
-      <c r="F89">
+      <c r="F89" s="1"/>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data import for NEDC
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/Taraba/test_services_excel.xlsx
+++ b/tests/testthat/testdata/Taraba/test_services_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admn\Documents\2-Biz\DevSolutions\clientele\JHPIEGO\jGBV\tests\testthat\testdata\Taraba\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22A73FC-C31B-4826-BABA-22EFCC872F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17096374-A32D-4B15-AC37-AF8B2926BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="24">
   <si>
     <t>agegp</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>rem3</t>
   </si>
 </sst>
 </file>
@@ -927,15 +933,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -960,8 +966,11 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -986,8 +995,11 @@
       <c r="H2">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1012,8 +1024,11 @@
       <c r="H3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1038,8 +1053,11 @@
       <c r="H4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1064,8 +1082,11 @@
       <c r="H5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1090,8 +1111,11 @@
       <c r="H6">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1116,8 +1140,11 @@
       <c r="H7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1142,8 +1169,11 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1168,8 +1198,11 @@
       <c r="H9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1194,8 +1227,11 @@
       <c r="H10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1220,8 +1256,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1246,8 +1285,11 @@
       <c r="H12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1263,14 +1305,20 @@
       <c r="E13" t="s">
         <v>7</v>
       </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1286,15 +1334,20 @@
       <c r="E14" s="1">
         <v>43739</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1310,14 +1363,20 @@
       <c r="E15" t="s">
         <v>8</v>
       </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1333,14 +1392,20 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1365,8 +1430,11 @@
       <c r="H17">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1391,8 +1459,11 @@
       <c r="H18">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1417,8 +1488,11 @@
       <c r="H19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1443,8 +1517,11 @@
       <c r="H20">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1469,8 +1546,11 @@
       <c r="H21">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1495,8 +1575,11 @@
       <c r="H22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1521,8 +1604,11 @@
       <c r="H23">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1547,8 +1633,11 @@
       <c r="H24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1573,8 +1662,11 @@
       <c r="H25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1599,8 +1691,11 @@
       <c r="H26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1625,8 +1720,11 @@
       <c r="H27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1651,8 +1749,11 @@
       <c r="H28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1668,14 +1769,20 @@
       <c r="E29" t="s">
         <v>7</v>
       </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="H29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1691,15 +1798,20 @@
       <c r="E30" s="1">
         <v>43739</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1715,14 +1827,20 @@
       <c r="E31" t="s">
         <v>8</v>
       </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1747,8 +1865,11 @@
       <c r="H32">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1773,8 +1894,11 @@
       <c r="H33">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1799,8 +1923,11 @@
       <c r="H34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1825,8 +1952,11 @@
       <c r="H35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1851,8 +1981,11 @@
       <c r="H36">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1877,8 +2010,11 @@
       <c r="H37">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1903,8 +2039,11 @@
       <c r="H38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1929,8 +2068,11 @@
       <c r="H39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1955,8 +2097,11 @@
       <c r="H40">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1981,8 +2126,11 @@
       <c r="H41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2007,8 +2155,11 @@
       <c r="H42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2033,8 +2184,11 @@
       <c r="H43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2050,14 +2204,20 @@
       <c r="E44" t="s">
         <v>7</v>
       </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
       <c r="G44">
         <v>4</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2073,15 +2233,20 @@
       <c r="E45" s="1">
         <v>43739</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
       <c r="G45">
         <v>3</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2097,14 +2262,20 @@
       <c r="E46" t="s">
         <v>8</v>
       </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
       <c r="G46">
         <v>2</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2120,14 +2291,20 @@
       <c r="E47" t="s">
         <v>9</v>
       </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
       <c r="G47">
         <v>4</v>
       </c>
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2152,8 +2329,11 @@
       <c r="H48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2178,8 +2358,11 @@
       <c r="H49">
         <v>19</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2204,8 +2387,11 @@
       <c r="H50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2230,8 +2416,11 @@
       <c r="H51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2256,8 +2445,11 @@
       <c r="H52">
         <v>31</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2282,8 +2474,11 @@
       <c r="H53">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2308,8 +2503,11 @@
       <c r="H54">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2334,8 +2532,11 @@
       <c r="H55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2360,8 +2561,11 @@
       <c r="H56">
         <v>9</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2386,8 +2590,11 @@
       <c r="H57">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2412,8 +2619,11 @@
       <c r="H58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2438,8 +2648,11 @@
       <c r="H59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2455,14 +2668,20 @@
       <c r="E60" t="s">
         <v>7</v>
       </c>
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
       <c r="G60">
         <v>5</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2478,15 +2697,20 @@
       <c r="E61" s="1">
         <v>43739</v>
       </c>
-      <c r="F61" s="1"/>
+      <c r="F61" t="s">
+        <v>22</v>
+      </c>
       <c r="G61">
         <v>6</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2502,14 +2726,20 @@
       <c r="E62" t="s">
         <v>8</v>
       </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
       <c r="G62">
         <v>2</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2525,14 +2755,20 @@
       <c r="E63" t="s">
         <v>9</v>
       </c>
+      <c r="F63" t="s">
+        <v>22</v>
+      </c>
       <c r="G63">
         <v>5</v>
       </c>
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2557,8 +2793,11 @@
       <c r="H64">
         <v>43</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2583,8 +2822,11 @@
       <c r="H65">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2609,8 +2851,11 @@
       <c r="H66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2635,8 +2880,11 @@
       <c r="H67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2661,8 +2909,11 @@
       <c r="H68">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2687,8 +2938,11 @@
       <c r="H69">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2713,8 +2967,11 @@
       <c r="H70">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2739,8 +2996,11 @@
       <c r="H71">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2765,8 +3025,11 @@
       <c r="H72">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2791,8 +3054,11 @@
       <c r="H73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2817,8 +3083,11 @@
       <c r="H74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2834,14 +3103,20 @@
       <c r="E75" t="s">
         <v>7</v>
       </c>
+      <c r="F75" t="s">
+        <v>22</v>
+      </c>
       <c r="G75">
         <v>3</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2857,15 +3132,20 @@
       <c r="E76" s="1">
         <v>43739</v>
       </c>
-      <c r="F76" s="1"/>
+      <c r="F76" t="s">
+        <v>22</v>
+      </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2881,14 +3161,20 @@
       <c r="E77" t="s">
         <v>8</v>
       </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
       <c r="G77">
         <v>1</v>
       </c>
       <c r="H77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2904,14 +3190,20 @@
       <c r="E78" t="s">
         <v>9</v>
       </c>
+      <c r="F78" t="s">
+        <v>22</v>
+      </c>
       <c r="G78">
         <v>1</v>
       </c>
       <c r="H78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2936,8 +3228,11 @@
       <c r="H79">
         <v>17</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2962,8 +3257,11 @@
       <c r="H80">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2988,8 +3286,11 @@
       <c r="H81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3014,8 +3315,11 @@
       <c r="H82">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3040,8 +3344,11 @@
       <c r="H83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3066,8 +3373,11 @@
       <c r="H84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3092,8 +3402,11 @@
       <c r="H85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3118,8 +3431,11 @@
       <c r="H86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3144,8 +3460,11 @@
       <c r="H87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <v>119119</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3161,14 +3480,20 @@
       <c r="E88" t="s">
         <v>7</v>
       </c>
+      <c r="F88" t="s">
+        <v>22</v>
+      </c>
       <c r="G88">
         <v>2</v>
       </c>
       <c r="H88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3184,15 +3509,23 @@
       <c r="E89" s="1">
         <v>43739</v>
       </c>
-      <c r="F89" s="1"/>
+      <c r="F89" t="s">
+        <v>22</v>
+      </c>
       <c r="G89">
         <v>1</v>
       </c>
       <c r="H89">
         <v>0</v>
       </c>
+      <c r="I89" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H90">
+    <sortCondition ref="A1:A90"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>